<commit_message>
Implementación lectura de datos desde excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/AutomationData.xlsx
+++ b/src/test/resources/data/AutomationData.xlsx
@@ -647,7 +647,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="220">
   <si>
     <t xml:space="preserve">Cedula</t>
   </si>
@@ -853,6 +853,9 @@
     <t xml:space="preserve">pais</t>
   </si>
   <si>
+    <t xml:space="preserve">ciudadExt</t>
+  </si>
+  <si>
     <t xml:space="preserve">monto</t>
   </si>
   <si>
@@ -955,292 +958,298 @@
     <t xml:space="preserve">ciudadRefF</t>
   </si>
   <si>
+    <t xml:space="preserve">"91077296"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"55857"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Soacha"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ANGEL MARIA MEJIA SANDOVAL"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"06/09/1979"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"3183903022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"aalvarez@excelcredit.co" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Pensionado"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Entidad donde trabaja"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"20000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"1.70"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"60"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"260000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"100000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"5500000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"300000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Compra de cartera"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"src/test/resources/Data/PDFPRUEBA.pdf" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"12345"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ANGEL"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"MARIA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"MEJIA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"SANDOVAL"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ANGEL MARIA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"18/01/1974" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"F"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Estrato 1" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Arriendo" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Casa" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Jefe de hogar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Universitario" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Desprendible de nómina" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"30000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Pago masivo (efectivo)" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"AAA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"colombia"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"colombiano"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Soltera/o"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ingeniero" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Antioquia"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Abejorral" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Cra 14 No. 93a - 30" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"24"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"2"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"pension"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"123456"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"01/01/2015"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"30/12/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"123456"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Certificación laboral"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"CEO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Luis Perez Ramirez"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"1234567890"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"No"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Importaciones"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Santander"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"966855"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Inversiones en oro" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Alemania"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Berlin" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"8500"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Euros"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"12/12/2008"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Febrero"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"20/07/1963"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Efectivo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"16/02/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Vinculado"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Plan 1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Si"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Juli Macias"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Prima"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"maria"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"camila"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"lopez"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"cardenas"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Amigo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"3204567894"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Arauca"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"juan"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"david"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"reyes"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"sanchez"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Hijo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"3204047804"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Amazonas"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Leticia"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retanqueo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"7500000"</t>
+  </si>
+  <si>
     <t xml:space="preserve">"10092369"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"55857"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Soacha"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"JAIRO MENDOZA DIAZ"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"19/10/1952"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"3183903022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"aalvarez@excelcredit.co" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Pensionado"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"P.A COLPENSIONES"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Entidad donde trabaja"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"20000000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"1.70"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"60"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"100"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"260000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"100000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"5500000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"300000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Retanqueo compra de cartera"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"src/test/resources/Data/PDFPRUEBA.pdf" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Pendientes por Radicar"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">""</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"12345"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"JAIRO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"MENDOZA" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DIAZ"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"18/01/1974" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"F"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Estrato 1" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Arriendo" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Casa" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Jefe de hogar"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Universitario" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Desprendible de nómina" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"30000000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Pago ma+AG1:AM2sivo (efectivo)" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"AAA"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"colombia"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"colombiano"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Soltera/o"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"ingeniero" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Antioquia"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Abejorral" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Cra 14 No. 93a - 30" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"24"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"2"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"0"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"pension"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"123456"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"01/01/2015"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"30/12/2022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"123456"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Certificación laboral"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"CEO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Luis Perez Ramirez"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"1234567890"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"No"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Importaciones"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Santander"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"966855"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Inversiones en oro" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Alemania"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Berlin" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"8500"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Euros"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"12/12/2008"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Febrero"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"20/07/1963"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"2022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Efectivo"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"16/02/2022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Vinculado"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Plan 1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Si"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Juli Macias"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Prima"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"maria"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"camila"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"lopez"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"cardenas"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Amigo"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"3204567894"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Arauca"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"juan"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"david"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"reyes"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"sanchez"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Hijo"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"3204047804"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Amazonas"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Leticia"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retanqueo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"7500000"</t>
   </si>
   <si>
     <t xml:space="preserve">"68003"</t>
@@ -1421,7 +1430,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1431,10 +1440,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1565,13 +1570,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CY3"/>
+  <dimension ref="A1:CY2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CU1" activeCellId="0" sqref="CU1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BQ1" activeCellId="0" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.01"/>
@@ -1633,7 +1638,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="17.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1839,174 +1844,174 @@
         <v>67</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BT1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BU1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BV1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BW1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BY1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="CA1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="CB1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CC1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CD1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="CE1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CF1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="CG1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CH1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CI1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="CJ1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="CK1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="CL1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CM1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CN1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="CO1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="CP1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="CQ1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="CR1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="CS1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="CT1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="CU1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="CV1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="CW1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="CX1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="CY1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="V2" s="0" t="s">
         <v>123</v>
@@ -2018,256 +2023,242 @@
         <v>125</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AT2" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AV2" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AW2" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AX2" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="BA2" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="BB2" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="BC2" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="BD2" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="BE2" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="BF2" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="BG2" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="BH2" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="BI2" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BJ2" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="BK2" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="BL2" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="BM2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="BN2" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="BO2" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="BP2" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="BQ2" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="BR2" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="BS2" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="BT2" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="BN2" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="BO2" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="BP2" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="BQ2" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="BR2" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="BS2" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="BT2" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="BU2" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="BV2" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="BW2" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="BX2" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="BY2" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="BZ2" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="CA2" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="CB2" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="CC2" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="CD2" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="CE2" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="CF2" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="CG2" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="CH2" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="CI2" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="CJ2" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="CK2" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="CL2" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="CM2" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="CN2" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="CO2" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="CP2" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="CQ2" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="CR2" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="CS2" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="CT2" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="CU2" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="CV2" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="CW2" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="CX2" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="CY2" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="W3" s="1"/>
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2295,11 +2286,11 @@
       <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2338,99 +2329,99 @@
         <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="H2" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>119</v>
+      <c r="F2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>204</v>
+        <v>150</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2468,7 +2459,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -2679,43 +2670,43 @@
         <v>46</v>
       </c>
       <c r="BR2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BS2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BT2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BU2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BV2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BW2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BX2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BY2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="CA2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="CB2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CC2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CD2" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,12 +2717,12 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste pesp y firma documentos codigo ado digicredito sin conflitos
</commit_message>
<xml_diff>
--- a/src/test/resources/data/AutomationData.xlsx
+++ b/src/test/resources/data/AutomationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\DigicreditoSerenity BDD\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28F4CB-CAB8-4C65-9932-AD952817C14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC27456-CE98-4649-B9CE-11C04DE919E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1875" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataDigicredito" sheetId="1" r:id="rId1"/>
@@ -2675,9 +2675,6 @@
     <t xml:space="preserve">"daabogadog@hotmail.com" </t>
   </si>
   <si>
-    <t>"3142739038"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> bancoInt       </t>
   </si>
   <si>
@@ -2690,34 +2687,37 @@
     <t>"COLFONDOS"</t>
   </si>
   <si>
-    <t>"5744075"</t>
-  </si>
-  <si>
-    <t>"DELIO"</t>
-  </si>
-  <si>
-    <t>"ARNULFO"</t>
-  </si>
-  <si>
-    <t>"ROJAS"</t>
-  </si>
-  <si>
     <t>"GUIO"</t>
   </si>
   <si>
     <t>"81768"</t>
   </si>
   <si>
-    <t>"DELIO ARNULFO ROJAS GUIO"</t>
-  </si>
-  <si>
-    <t>"Retanqueo compra de cartera"</t>
-  </si>
-  <si>
     <t>"14/03/2022"</t>
   </si>
   <si>
     <t>"14/Mar/2022"</t>
+  </si>
+  <si>
+    <t>"98466617"</t>
+  </si>
+  <si>
+    <t>"CARLOS"</t>
+  </si>
+  <si>
+    <t>"EDUARDO"</t>
+  </si>
+  <si>
+    <t>"FERIA"</t>
+  </si>
+  <si>
+    <t>"CARLOS EDUARDO FERIA"</t>
+  </si>
+  <si>
+    <t>"Libre inversion"</t>
+  </si>
+  <si>
+    <t>"3132739036"</t>
   </si>
 </sst>
 </file>
@@ -3480,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3665,7 +3665,7 @@
         <v>202</v>
       </c>
       <c r="AN1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AO1" t="s">
         <v>203</v>
@@ -3794,7 +3794,7 @@
         <v>244</v>
       </c>
       <c r="CE1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="CF1" t="s">
         <v>245</v>
@@ -3904,10 +3904,10 @@
     </row>
     <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>296</v>
@@ -3916,7 +3916,7 @@
         <v>146</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>146</v>
@@ -3934,22 +3934,22 @@
         <v>303</v>
       </c>
       <c r="K2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="P2" t="s">
         <v>312</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="P2" t="s">
-        <v>319</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>82</v>
@@ -3961,7 +3961,7 @@
         <v>279</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>280</v>
@@ -3973,7 +3973,7 @@
         <v>304</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="Y2" s="6" t="s">
         <v>282</v>
@@ -4039,10 +4039,10 @@
         <v>100</v>
       </c>
       <c r="AT2" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="AU2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AV2" s="11" t="s">
         <v>163</v>
@@ -4051,7 +4051,7 @@
         <v>85</v>
       </c>
       <c r="AX2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AY2" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
ajuste flujo de digicredito
</commit_message>
<xml_diff>
--- a/src/test/resources/data/AutomationData.xlsx
+++ b/src/test/resources/data/AutomationData.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\DigicreditoSerenity BDD\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F19613A-ACC9-464F-898D-942C22929D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE74C4A-0F74-433C-AF8C-6E81E2805278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1875" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataDigicredito" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -60,7 +60,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Monto solicitado para el Retanqueo;
 *No debe contener puntos ni comas</t>
@@ -85,7 +85,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cedula del cliente
 *No debe contener puntos ni comas</t>
@@ -110,7 +110,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero indentificador de el credito al cual posteriormente se va a realizar un Retanqueo.
 Es importante verificar el estado del credito en curso por consulta a base de datos.</t>
@@ -135,7 +135,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ruta o Path en la cual se almacena el PDF para pruebas de carga de documentos;
 *Verificar su existencia antes de lanzar una prueba</t>
@@ -160,7 +160,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tasa del Crédito;
 *Debe siempre estar a dos decimales.
@@ -187,7 +187,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Plazo en meses del crédito
 </t>
@@ -212,7 +212,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Días hábiles de intereses iniciales</t>
         </r>
@@ -236,7 +236,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ingresos del cliente;
 *Debe estar sin puntos ni comas</t>
@@ -261,7 +261,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Descuentos de Ley;
 *Sin puntos ni comas</t>
@@ -286,7 +286,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Descuento de nomina;
 *Sin puntos ni comas</t>
@@ -311,7 +311,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valor total por la suma de las compras y saneamientos que se le van a recoger al cliente;
 *Sin puntos ni comas</t>
@@ -336,7 +336,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -360,7 +360,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nombre del Crédito;
 *Se recomienda usar el primer nombre del Cliente</t>
@@ -385,7 +385,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Mes en el cual se va a lanzar la Originación;
 *Siempre mes Actual
@@ -411,7 +411,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Año de nacimiento del cliente;
 *Debe estar en formato:
@@ -439,7 +439,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Año actual.
 *Formato;
@@ -465,7 +465,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero Celular del Cliente;
 *Para pruebas automatizadas cambiar el celular desde bases de datos por uno de prueba</t>
@@ -490,7 +490,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Correo electrónico del Cliente;
 *Para pruebas automatizadas cambiar el correo desde bases de datos por uno de prueba</t>
@@ -515,7 +515,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tipo de desembolso del crédito.
 *Debe coincidir con las opciones del sistema</t>
@@ -540,7 +540,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha Actual
 *Formato de fecha:
@@ -568,7 +568,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -592,7 +592,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero de radicación de la solicitud.
 Consultarlo en base de datos.</t>
@@ -604,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="359">
   <si>
     <t>Cedula</t>
   </si>
@@ -1269,359 +1269,425 @@
     <t xml:space="preserve"> Banco                             </t>
   </si>
   <si>
-    <t xml:space="preserve"> "P.A COLPENSIONES" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3994518" </t>
+    <t xml:space="preserve">"P.A COLPENSIONES" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "8500000" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"250000" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Pensionado" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"20500000"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Jubilados"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "10/03/2000" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Cundinamarca" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Anapoima" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"src/test/resources/Data/PDFPRUEBA.pdf" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Educacion propia" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "M"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Soltera/o" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Calle 2d #22-52"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Arriendo"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"perez"             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "alejandro"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "7210273"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "9007146"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3112" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2022"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Efectivo" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "'ACRED','EGRESO'" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "upper('Desembolso egreso'), upper('Desembolso activación de crédito')" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "15/02/1956"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Entidad donde trabaja" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ""           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ""   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "12345" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "06/08/1976"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Estrato 1" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Casa"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Jefe de hogar" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Universitario"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "100000"         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Desprendible de nómina" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "5000000"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Pago masivo (efectivo)" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "AAA"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "colombia"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "colombia"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "colombiano" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ingeniero" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "24"            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2"         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "0"            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "pension"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "123456"             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "30/12/2022"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "123456"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Certificación laboral" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "CEO" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Luis Perez Ramirez" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "1234567890"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3183903022"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Importaciones"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Santander" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "966855"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Inversiones en oro" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Alemania" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Berlin"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "8500" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Euros" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "12/12/2008"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Febrero" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "20/07/1963" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2022"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "16/02/2022" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Vinculado" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Plan 1" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Si"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Juli Macias"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Prima"            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "maria"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "camila"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "lopez"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "cardenas"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Amigo"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3204567894" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "juan"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "david"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "reyes"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "sanchez"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Hijo"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3204047804" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Pensionado por Invalidez" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"3994518" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "1.71" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"60"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"30500000"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"90"                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"200000"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Abril" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"14/04/2022"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "SERGIO"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "SEGUNDO"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "URZOLA"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "BERTEL"        </t>
+  </si>
+  <si>
+    <t>"05/04/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Florencia"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"600000"              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "lespitiameza@gmail.com" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3219176522" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29/10/2021    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"600000"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "DELIO ARNULFO ROJAS GUIO" </t>
+  </si>
+  <si>
+    <t>"Compra de cartera"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"14206887" </t>
   </si>
   <si>
     <t xml:space="preserve"> "1.70" </t>
   </si>
   <si>
-    <t xml:space="preserve"> "16"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "90"                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "8500000" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "250000" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "300000"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Marzo" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "14/03/2022"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "SERGIO"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "SEGUNDO"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "URZOLA"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "BERTEL"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "18/Mar/2022" </t>
+    <t xml:space="preserve">"24"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"40500000"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"60"                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"300000"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Marzo" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"14/03/2022"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "JOSE"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "DEL CARMEN"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "VILLARREAL"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "GONZALEZ"        </t>
+  </si>
+  <si>
+    <t>"30/03/2022"</t>
   </si>
   <si>
     <t xml:space="preserve"> "Soacha"      </t>
   </si>
   <si>
-    <t xml:space="preserve"> "Pensionado" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "20500000"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "500000"              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Jubilados"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "10/03/2000" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "lespitiameza@gmail.com" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3219176522" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cundinamarca" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Anapoima" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "src/test/resources/Data/PDFPRUEBA.pdf" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Educacion propia" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "M"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Soltera/o" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Calle 2d #22-52"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Arriendo"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "perez"             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "alejandro"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "7210273"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "9007146"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3112" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2022"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Efectivo" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "'ACRED','EGRESO'" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "upper('Desembolso egreso'), upper('Desembolso activación de crédito')" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 29/10/2021    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "0"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "0"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "81768" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "DELIO ARNULFO ROJAS GUIO" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "15/02/1956"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Entidad donde trabaja" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Compra de cartera" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ""           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ""   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "12345" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "06/08/1976"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Estrato 1" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Casa"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Jefe de hogar" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Universitario"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "100000"         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Desprendible de nómina" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "5000000"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Pago masivo (efectivo)" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "AAA"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "colombia"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "colombia"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "colombiano" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "ingeniero" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "24"            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2"         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "0"            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "pension"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "123456"             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "30/12/2022"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "123456"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Certificación laboral" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "CEO" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Luis Perez Ramirez" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "1234567890"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3183903022"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Importaciones"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Santander" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "966855"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Inversiones en oro" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Alemania" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Berlin"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "8500" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Euros" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"               </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "12/12/2008"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Febrero" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "20/07/1963" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2022"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "16/02/2022" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Vinculado" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Plan 1" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Si"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Juli Macias"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Prima"            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "maria"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "camila"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "lopez"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "cardenas"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Amigo"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3204567894" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "juan"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "david"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "reyes"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "sanchez"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hijo"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3204047804" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "92875"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Pensionado por Invalidez" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "1500000"      </t>
+    <t xml:space="preserve">"0"              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "daabogadog@gmail.com" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"3132739036" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29/10/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"85900" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "JOSE DEL CARMEN VILLARREAL GONZALEZ" </t>
+  </si>
+  <si>
+    <t>"Libre inversion"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"92947"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "92948"       </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1633,7 +1699,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1657,6 +1723,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1678,12 +1757,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1692,7 +1786,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1703,13 +1797,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Neutral" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2128,16 +2236,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DN2"/>
+  <dimension ref="A1:DN3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
@@ -2157,7 +2265,7 @@
     <col min="20" max="20" width="39.7109375" customWidth="1"/>
     <col min="21" max="21" width="23.42578125" customWidth="1"/>
     <col min="22" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" customWidth="1"/>
+    <col min="23" max="23" width="31" customWidth="1"/>
     <col min="24" max="24" width="14.28515625" customWidth="1"/>
     <col min="25" max="25" width="15.85546875" customWidth="1"/>
     <col min="26" max="26" width="14.5703125" customWidth="1"/>
@@ -2183,7 +2291,7 @@
     <col min="47" max="47" width="16.5703125" customWidth="1"/>
     <col min="48" max="48" width="19.140625" customWidth="1"/>
     <col min="49" max="49" width="16.42578125" customWidth="1"/>
-    <col min="50" max="50" width="15.28515625" customWidth="1"/>
+    <col min="50" max="50" width="37.140625" customWidth="1"/>
     <col min="51" max="51" width="11.7109375" customWidth="1"/>
     <col min="52" max="52" width="22.5703125" customWidth="1"/>
     <col min="53" max="53" width="12.42578125" customWidth="1"/>
@@ -2556,361 +2664,720 @@
       <c r="A2" t="s">
         <v>221</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G2" t="s">
         <v>222</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>223</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2" t="s">
+        <v>319</v>
+      </c>
+      <c r="K2" t="s">
+        <v>320</v>
+      </c>
+      <c r="L2" t="s">
+        <v>321</v>
+      </c>
+      <c r="M2" t="s">
+        <v>322</v>
+      </c>
+      <c r="N2" t="s">
+        <v>323</v>
+      </c>
+      <c r="O2" t="s">
+        <v>324</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>326</v>
+      </c>
+      <c r="R2" t="s">
         <v>224</v>
       </c>
-      <c r="E2" t="s">
+      <c r="S2" t="s">
+        <v>225</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="U2" t="s">
+        <v>226</v>
+      </c>
+      <c r="V2" t="s">
+        <v>227</v>
+      </c>
+      <c r="W2" t="s">
+        <v>328</v>
+      </c>
+      <c r="X2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>244</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>330</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="AS2" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="AT2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>247</v>
+      </c>
+      <c r="AX2" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>251</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>252</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>253</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>255</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>257</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>258</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>259</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>260</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>264</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>265</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>266</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>267</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>268</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>269</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>270</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>271</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>273</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>274</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>276</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>277</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>278</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>277</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>279</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>280</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>281</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>282</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>283</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>284</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>285</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>286</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>277</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>287</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>288</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>289</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>290</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>291</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>293</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>294</v>
+      </c>
+      <c r="CV2" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="CW2" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>297</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>298</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>299</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>300</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>301</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>302</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>303</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>304</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>305</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>306</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>307</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>308</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>309</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>310</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>311</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>357</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" t="s">
         <v>336</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E3" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I3" t="s">
+        <v>340</v>
+      </c>
+      <c r="J3" t="s">
+        <v>341</v>
+      </c>
+      <c r="K3" t="s">
+        <v>342</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>348</v>
+      </c>
+      <c r="R3" t="s">
+        <v>224</v>
+      </c>
+      <c r="S3" t="s">
         <v>225</v>
       </c>
-      <c r="G2" t="s">
+      <c r="T3" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="U3" t="s">
         <v>226</v>
       </c>
-      <c r="H2" t="s">
+      <c r="V3" t="s">
         <v>227</v>
       </c>
-      <c r="I2" t="s">
+      <c r="W3" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="Y3" t="s">
         <v>228</v>
       </c>
-      <c r="J2" t="s">
+      <c r="Z3" t="s">
         <v>229</v>
       </c>
-      <c r="K2" t="s">
+      <c r="AA3" t="s">
         <v>230</v>
       </c>
-      <c r="L2" t="s">
+      <c r="AB3" t="s">
         <v>231</v>
       </c>
-      <c r="M2" t="s">
+      <c r="AC3" t="s">
         <v>232</v>
       </c>
-      <c r="N2" t="s">
+      <c r="AD3" t="s">
         <v>233</v>
       </c>
-      <c r="O2" t="s">
+      <c r="AE3" t="s">
         <v>234</v>
       </c>
-      <c r="P2" t="s">
+      <c r="AF3" t="s">
         <v>235</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AG3" t="s">
         <v>236</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AH3" t="s">
         <v>237</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AI3" t="s">
         <v>238</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AJ3" t="s">
         <v>239</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AK3" t="s">
         <v>240</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AL3" t="s">
         <v>241</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AM3" t="s">
         <v>242</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AN3" t="s">
         <v>243</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AO3" t="s">
         <v>244</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AP3" t="s">
         <v>245</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AQ3" t="s">
+        <v>352</v>
+      </c>
+      <c r="AR3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS3" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AU3" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="AV3" t="s">
         <v>246</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AW3" t="s">
         <v>247</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AX3" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="AY3" t="s">
         <v>248</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AZ3" t="s">
         <v>249</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="BA3" t="s">
         <v>250</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="BB3" t="s">
         <v>251</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="BC3" t="s">
         <v>252</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="BD3" t="s">
         <v>253</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="BE3" t="s">
         <v>254</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="BF3" t="s">
         <v>255</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="BG3" t="s">
         <v>256</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="BH3" t="s">
         <v>257</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="BI3" t="s">
         <v>258</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="BJ3" t="s">
         <v>259</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="BK3" t="s">
         <v>260</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="BL3" t="s">
         <v>261</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="BM3" t="s">
         <v>262</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="BN3" t="s">
         <v>263</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="BO3" t="s">
         <v>264</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="BP3" t="s">
         <v>265</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BQ3" t="s">
         <v>266</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BR3" t="s">
         <v>267</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BS3" t="s">
         <v>268</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BT3" t="s">
         <v>269</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BU3" t="s">
         <v>270</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BV3" t="s">
         <v>271</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BW3" t="s">
         <v>272</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BX3" t="s">
         <v>273</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BY3" t="s">
         <v>274</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BZ3" t="s">
         <v>275</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="CA3" t="s">
         <v>276</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="CB3" t="s">
         <v>277</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="CC3" t="s">
         <v>278</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="CD3" t="s">
+        <v>277</v>
+      </c>
+      <c r="CE3" t="s">
         <v>279</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="CF3" t="s">
         <v>280</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="CG3" t="s">
         <v>281</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="CH3" t="s">
         <v>282</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="CI3" t="s">
         <v>283</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="CJ3" t="s">
         <v>284</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="CK3" t="s">
         <v>285</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="CL3" t="s">
         <v>286</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="CM3" t="s">
+        <v>277</v>
+      </c>
+      <c r="CN3" t="s">
         <v>287</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="CO3" t="s">
         <v>288</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="CP3" t="s">
         <v>289</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="CQ3" t="s">
         <v>290</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="CR3" t="s">
         <v>291</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="CS3" t="s">
         <v>292</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="CT3" t="s">
         <v>293</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CU3" t="s">
         <v>294</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CV3" t="s">
         <v>295</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CW3" t="s">
         <v>296</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CX3" t="s">
         <v>297</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CY3" t="s">
         <v>298</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CZ3" t="s">
         <v>299</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="DA3" t="s">
         <v>300</v>
       </c>
-      <c r="CD2" t="s">
-        <v>299</v>
-      </c>
-      <c r="CE2" t="s">
+      <c r="DB3" t="s">
         <v>301</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="DC3" t="s">
         <v>302</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="DD3" t="s">
         <v>303</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="DE3" t="s">
         <v>304</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="DF3" t="s">
         <v>305</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="DG3" t="s">
         <v>306</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="DH3" t="s">
         <v>307</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="DI3" t="s">
         <v>308</v>
       </c>
-      <c r="CM2" t="s">
-        <v>299</v>
-      </c>
-      <c r="CN2" t="s">
+      <c r="DJ3" t="s">
         <v>309</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="DK3" t="s">
         <v>310</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="DL3" t="s">
         <v>311</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="DM3" t="s">
+        <v>358</v>
+      </c>
+      <c r="DN3" t="s">
         <v>312</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>313</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>314</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>315</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>316</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>317</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>318</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>319</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>320</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>321</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>322</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>323</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>324</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>325</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>326</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>327</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>328</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>329</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>330</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>331</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>332</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>333</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>334</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>335</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="3" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="148"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>